<commit_message>
plot cleanup / update
</commit_message>
<xml_diff>
--- a/Analysis/Data/final/GAS-004/XRD+synthsis_data.xlsx
+++ b/Analysis/Data/final/GAS-004/XRD+synthsis_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\queim\Documents\CARES\Github\RAHMBO\Analysis\Data\final\GAS-004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EB2E5F-4E1C-4496-B848-DBE7860FD7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22104D61-AAC1-4048-994C-93B6258B4F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-60" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
   <dimension ref="A1:W103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="K1" sqref="K1:K103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +872,7 @@
         <v>2.3199999332427979</v>
       </c>
       <c r="K2">
-        <v>0.1354080076260567</v>
+        <v>0.99299205054378525</v>
       </c>
       <c r="L2">
         <v>387.99006048968931</v>
@@ -943,7 +943,7 @@
         <v>2.3199999332427979</v>
       </c>
       <c r="K3">
-        <v>0.1354080076260567</v>
+        <v>0.99299205054378525</v>
       </c>
       <c r="L3">
         <v>387.99006048968931</v>
@@ -1014,7 +1014,7 @@
         <v>2.3199999332427979</v>
       </c>
       <c r="K4">
-        <v>0.1354080076260567</v>
+        <v>0.99299205054378525</v>
       </c>
       <c r="L4">
         <v>387.99006048968931</v>
@@ -1085,7 +1085,7 @@
         <v>1.0900000333786011</v>
       </c>
       <c r="K5">
-        <v>0.7246799985837924</v>
+        <v>6.0389999881982703</v>
       </c>
       <c r="L5">
         <v>238.03279180611329</v>
@@ -1156,7 +1156,7 @@
         <v>1.0900000333786011</v>
       </c>
       <c r="K6">
-        <v>0.7246799985837924</v>
+        <v>6.0389999881982703</v>
       </c>
       <c r="L6">
         <v>238.03279180611329</v>
@@ -1227,7 +1227,7 @@
         <v>1.0900000333786011</v>
       </c>
       <c r="K7">
-        <v>0.7246799985837924</v>
+        <v>6.0389999881982703</v>
       </c>
       <c r="L7">
         <v>238.03279180611329</v>
@@ -1298,7 +1298,7 @@
         <v>1.929999947547913</v>
       </c>
       <c r="K8">
-        <v>0.57131522431526216</v>
+        <v>2.380480101313593</v>
       </c>
       <c r="L8">
         <v>276.06936244116372</v>
@@ -1369,7 +1369,7 @@
         <v>1.929999947547913</v>
       </c>
       <c r="K9">
-        <v>0.57131522431526216</v>
+        <v>2.380480101313593</v>
       </c>
       <c r="L9">
         <v>276.06936244116372</v>
@@ -1440,7 +1440,7 @@
         <v>1.929999947547913</v>
       </c>
       <c r="K10">
-        <v>0.57131522431526216</v>
+        <v>2.380480101313593</v>
       </c>
       <c r="L10">
         <v>276.06936244116372</v>
@@ -1511,7 +1511,7 @@
         <v>1.6599999666213989</v>
       </c>
       <c r="K11">
-        <v>0.48286798279953019</v>
+        <v>4.0238998566627524</v>
       </c>
       <c r="L11">
         <v>256.88213159388289</v>
@@ -1582,7 +1582,7 @@
         <v>1.6599999666213989</v>
       </c>
       <c r="K12">
-        <v>0.48286798279953019</v>
+        <v>4.0238998566627524</v>
       </c>
       <c r="L12">
         <v>256.88213159388289</v>
@@ -1653,7 +1653,7 @@
         <v>1.6599999666213989</v>
       </c>
       <c r="K13">
-        <v>0.48286798279953019</v>
+        <v>4.0238998566627524</v>
       </c>
       <c r="L13">
         <v>256.88213159388289</v>
@@ -1724,7 +1724,7 @@
         <v>1.470000028610229</v>
       </c>
       <c r="K14">
-        <v>0.39815997399330172</v>
+        <v>2.02397991526365</v>
       </c>
       <c r="L14">
         <v>233.92405613399731</v>
@@ -1795,7 +1795,7 @@
         <v>1.470000028610229</v>
       </c>
       <c r="K15">
-        <v>0.39815997399330172</v>
+        <v>2.02397991526365</v>
       </c>
       <c r="L15">
         <v>233.92405613399731</v>
@@ -1866,7 +1866,7 @@
         <v>1.470000028610229</v>
       </c>
       <c r="K16">
-        <v>0.39815997399330172</v>
+        <v>2.02397991526365</v>
       </c>
       <c r="L16">
         <v>233.92405613399731</v>
@@ -1937,7 +1937,7 @@
         <v>1.950000047683716</v>
       </c>
       <c r="K17">
-        <v>0.57362398951148974</v>
+        <v>4.7801999125957479</v>
       </c>
       <c r="L17">
         <v>330.11673697541067</v>
@@ -2008,7 +2008,7 @@
         <v>1.950000047683716</v>
       </c>
       <c r="K18">
-        <v>0.57362398951148974</v>
+        <v>4.7801999125957479</v>
       </c>
       <c r="L18">
         <v>330.11673697541067</v>
@@ -2079,7 +2079,7 @@
         <v>1.950000047683716</v>
       </c>
       <c r="K19">
-        <v>0.57362398951148974</v>
+        <v>4.7801999125957479</v>
       </c>
       <c r="L19">
         <v>330.11673697541067</v>
@@ -2150,7 +2150,7 @@
         <v>1.2899999618530269</v>
       </c>
       <c r="K20">
-        <v>0.63503998437881481</v>
+        <v>3.8102400576782189</v>
       </c>
       <c r="L20">
         <v>262.85714393840618</v>
@@ -2221,7 +2221,7 @@
         <v>1.2899999618530269</v>
       </c>
       <c r="K21">
-        <v>0.63503998437881481</v>
+        <v>3.8102400576782189</v>
       </c>
       <c r="L21">
         <v>262.85714393840618</v>
@@ -2292,7 +2292,7 @@
         <v>1.2899999618530269</v>
       </c>
       <c r="K22">
-        <v>0.63503998437881481</v>
+        <v>3.8102400576782189</v>
       </c>
       <c r="L22">
         <v>262.85714393840618</v>
@@ -2363,7 +2363,7 @@
         <v>2.309999942779541</v>
       </c>
       <c r="K23">
-        <v>6.9720000352263431E-2</v>
+        <v>0.58100000293552856</v>
       </c>
       <c r="L23">
         <v>305.88640458459639</v>
@@ -2434,7 +2434,7 @@
         <v>2.309999942779541</v>
       </c>
       <c r="K24">
-        <v>6.9720000352263431E-2</v>
+        <v>0.58100000293552856</v>
       </c>
       <c r="L24">
         <v>305.88640458459639</v>
@@ -2505,7 +2505,7 @@
         <v>2.309999942779541</v>
       </c>
       <c r="K25">
-        <v>6.9720000352263431E-2</v>
+        <v>0.58100000293552856</v>
       </c>
       <c r="L25">
         <v>305.88640458459639</v>
@@ -2576,7 +2576,7 @@
         <v>2.0499999523162842</v>
       </c>
       <c r="K26">
-        <v>9.9122399499606953E-2</v>
+        <v>0.4130099979150289</v>
       </c>
       <c r="L26">
         <v>272.97450548913201</v>
@@ -2647,7 +2647,7 @@
         <v>2.0499999523162842</v>
       </c>
       <c r="K27">
-        <v>9.9122399499606953E-2</v>
+        <v>0.4130099979150289</v>
       </c>
       <c r="L27">
         <v>272.97450548913201</v>
@@ -2718,7 +2718,7 @@
         <v>2.0499999523162842</v>
       </c>
       <c r="K28">
-        <v>9.9122399499606953E-2</v>
+        <v>0.4130099979150289</v>
       </c>
       <c r="L28">
         <v>272.97450548913201</v>
@@ -2789,7 +2789,7 @@
         <v>1.5399999618530269</v>
       </c>
       <c r="K29">
-        <v>0.56086800196838338</v>
+        <v>4.673900016403195</v>
       </c>
       <c r="L29">
         <v>297.92421243118361</v>
@@ -2860,7 +2860,7 @@
         <v>1.5399999618530269</v>
       </c>
       <c r="K30">
-        <v>0.56086800196838338</v>
+        <v>4.673900016403195</v>
       </c>
       <c r="L30">
         <v>297.92421243118361</v>
@@ -2931,7 +2931,7 @@
         <v>1.5399999618530269</v>
       </c>
       <c r="K31">
-        <v>0.56086800196838338</v>
+        <v>4.673900016403195</v>
       </c>
       <c r="L31">
         <v>297.92421243118361</v>
@@ -3002,7 +3002,7 @@
         <v>2.2000000476837158</v>
       </c>
       <c r="K32">
-        <v>1.1748239959487909</v>
+        <v>9.7901999662399248</v>
       </c>
       <c r="L32">
         <v>228.10811058498331</v>
@@ -3073,7 +3073,7 @@
         <v>2.2000000476837158</v>
       </c>
       <c r="K33">
-        <v>1.1748239959487909</v>
+        <v>9.7901999662399248</v>
       </c>
       <c r="L33">
         <v>228.10811058498331</v>
@@ -3144,7 +3144,7 @@
         <v>2.2000000476837158</v>
       </c>
       <c r="K34">
-        <v>1.1748239959487909</v>
+        <v>9.7901999662399248</v>
       </c>
       <c r="L34">
         <v>228.10811058498331</v>
@@ -3215,7 +3215,7 @@
         <v>1.200000047683716</v>
       </c>
       <c r="K35">
-        <v>0.22838399697875961</v>
+        <v>1.9031999748229971</v>
       </c>
       <c r="L35">
         <v>341.31147021985907</v>
@@ -3286,7 +3286,7 @@
         <v>1.200000047683716</v>
       </c>
       <c r="K36">
-        <v>0.22838399697875961</v>
+        <v>1.9031999748229971</v>
       </c>
       <c r="L36">
         <v>341.31147021985907</v>
@@ -3357,7 +3357,7 @@
         <v>1.200000047683716</v>
       </c>
       <c r="K37">
-        <v>0.22838399697875961</v>
+        <v>1.9031999748229971</v>
       </c>
       <c r="L37">
         <v>341.31147021985907</v>
@@ -3428,7 +3428,7 @@
         <v>1.23</v>
       </c>
       <c r="K38">
-        <v>8.32</v>
+        <v>8.3159999999999989</v>
       </c>
       <c r="L38">
         <v>234.29</v>
@@ -3499,7 +3499,7 @@
         <v>1.23</v>
       </c>
       <c r="K39">
-        <v>8.32</v>
+        <v>8.3159999999999989</v>
       </c>
       <c r="L39">
         <v>234.29</v>
@@ -3570,7 +3570,7 @@
         <v>1.23</v>
       </c>
       <c r="K40">
-        <v>8.32</v>
+        <v>8.3159999999999989</v>
       </c>
       <c r="L40">
         <v>234.29</v>
@@ -3641,7 +3641,7 @@
         <v>1.91</v>
       </c>
       <c r="K41">
-        <v>3.24</v>
+        <v>3.2448000000000001</v>
       </c>
       <c r="L41">
         <v>333.02</v>
@@ -3712,7 +3712,7 @@
         <v>1.91</v>
       </c>
       <c r="K42">
-        <v>3.24</v>
+        <v>3.2448000000000001</v>
       </c>
       <c r="L42">
         <v>333.02</v>
@@ -3783,7 +3783,7 @@
         <v>1.91</v>
       </c>
       <c r="K43">
-        <v>3.24</v>
+        <v>3.2448000000000001</v>
       </c>
       <c r="L43">
         <v>333.02</v>
@@ -3854,7 +3854,7 @@
         <v>1.02</v>
       </c>
       <c r="K44">
-        <v>4.37</v>
+        <v>4.3724999999999996</v>
       </c>
       <c r="L44">
         <v>250.91</v>
@@ -3925,7 +3925,7 @@
         <v>1.02</v>
       </c>
       <c r="K45">
-        <v>4.37</v>
+        <v>4.3724999999999996</v>
       </c>
       <c r="L45">
         <v>250.91</v>
@@ -3996,7 +3996,7 @@
         <v>1.02</v>
       </c>
       <c r="K46">
-        <v>4.37</v>
+        <v>4.3724999999999996</v>
       </c>
       <c r="L46">
         <v>250.91</v>
@@ -4280,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="K50">
-        <v>4.32</v>
+        <v>4.3179999999999996</v>
       </c>
       <c r="L50">
         <v>290.08</v>
@@ -4351,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="K51">
-        <v>4.32</v>
+        <v>4.3179999999999996</v>
       </c>
       <c r="L51">
         <v>290.08</v>
@@ -4422,7 +4422,7 @@
         <v>1</v>
       </c>
       <c r="K52">
-        <v>4.32</v>
+        <v>4.3179999999999996</v>
       </c>
       <c r="L52">
         <v>290.08</v>
@@ -4493,7 +4493,7 @@
         <v>1.47</v>
       </c>
       <c r="K53">
-        <v>1.89</v>
+        <v>1.8927</v>
       </c>
       <c r="L53">
         <v>274.07</v>
@@ -4564,7 +4564,7 @@
         <v>1.47</v>
       </c>
       <c r="K54">
-        <v>1.89</v>
+        <v>1.8927</v>
       </c>
       <c r="L54">
         <v>274.07</v>
@@ -4635,7 +4635,7 @@
         <v>1.47</v>
       </c>
       <c r="K55">
-        <v>1.89</v>
+        <v>1.8927</v>
       </c>
       <c r="L55">
         <v>274.07</v>
@@ -4706,7 +4706,7 @@
         <v>1</v>
       </c>
       <c r="K56">
-        <v>1.07</v>
+        <v>1.0746</v>
       </c>
       <c r="L56">
         <v>300.89999999999998</v>
@@ -4777,7 +4777,7 @@
         <v>1</v>
       </c>
       <c r="K57">
-        <v>1.07</v>
+        <v>1.0746</v>
       </c>
       <c r="L57">
         <v>300.89999999999998</v>
@@ -4848,7 +4848,7 @@
         <v>1</v>
       </c>
       <c r="K58">
-        <v>1.07</v>
+        <v>1.0746</v>
       </c>
       <c r="L58">
         <v>300.89999999999998</v>
@@ -4919,7 +4919,7 @@
         <v>1.82</v>
       </c>
       <c r="K59">
-        <v>1.4</v>
+        <v>1.3960999999999999</v>
       </c>
       <c r="L59">
         <v>297.92</v>
@@ -4990,7 +4990,7 @@
         <v>1.82</v>
       </c>
       <c r="K60">
-        <v>1.4</v>
+        <v>1.3960999999999999</v>
       </c>
       <c r="L60">
         <v>297.92</v>
@@ -5061,7 +5061,7 @@
         <v>1.82</v>
       </c>
       <c r="K61">
-        <v>1.4</v>
+        <v>1.3960999999999999</v>
       </c>
       <c r="L61">
         <v>297.92</v>
@@ -5132,7 +5132,7 @@
         <v>1.85</v>
       </c>
       <c r="K62">
-        <v>0.96</v>
+        <v>0.95620000000000038</v>
       </c>
       <c r="L62">
         <v>278.13</v>
@@ -5203,7 +5203,7 @@
         <v>1.85</v>
       </c>
       <c r="K63">
-        <v>0.96</v>
+        <v>0.95620000000000038</v>
       </c>
       <c r="L63">
         <v>278.13</v>
@@ -5274,7 +5274,7 @@
         <v>1.85</v>
       </c>
       <c r="K64">
-        <v>0.96</v>
+        <v>0.95620000000000038</v>
       </c>
       <c r="L64">
         <v>278.13</v>
@@ -5345,7 +5345,7 @@
         <v>2.5</v>
       </c>
       <c r="K65">
-        <v>8</v>
+        <v>8.0000000000000018</v>
       </c>
       <c r="L65">
         <v>228</v>
@@ -5416,7 +5416,7 @@
         <v>2.5</v>
       </c>
       <c r="K66">
-        <v>8</v>
+        <v>8.0000000000000018</v>
       </c>
       <c r="L66">
         <v>228</v>
@@ -5487,7 +5487,7 @@
         <v>2.5</v>
       </c>
       <c r="K67">
-        <v>8</v>
+        <v>8.0000000000000018</v>
       </c>
       <c r="L67">
         <v>228</v>
@@ -5558,7 +5558,7 @@
         <v>1.72</v>
       </c>
       <c r="K68">
-        <v>1.78</v>
+        <v>1.7842</v>
       </c>
       <c r="L68">
         <v>253.17</v>
@@ -5629,7 +5629,7 @@
         <v>1.72</v>
       </c>
       <c r="K69">
-        <v>1.78</v>
+        <v>1.7842</v>
       </c>
       <c r="L69">
         <v>253.17</v>
@@ -5700,7 +5700,7 @@
         <v>1.72</v>
       </c>
       <c r="K70">
-        <v>1.78</v>
+        <v>1.7842</v>
       </c>
       <c r="L70">
         <v>253.17</v>
@@ -5771,7 +5771,7 @@
         <v>2.38</v>
       </c>
       <c r="K71">
-        <v>3.74</v>
+        <v>3.7349999999999999</v>
       </c>
       <c r="L71">
         <v>250.12</v>
@@ -5842,7 +5842,7 @@
         <v>2.38</v>
       </c>
       <c r="K72">
-        <v>3.74</v>
+        <v>3.7349999999999999</v>
       </c>
       <c r="L72">
         <v>250.12</v>
@@ -5913,7 +5913,7 @@
         <v>2.38</v>
       </c>
       <c r="K73">
-        <v>3.74</v>
+        <v>3.7349999999999999</v>
       </c>
       <c r="L73">
         <v>250.12</v>
@@ -5984,7 +5984,7 @@
         <v>2.38</v>
       </c>
       <c r="K74">
-        <v>1.28</v>
+        <v>1.2834000000000001</v>
       </c>
       <c r="L74">
         <v>271.47000000000003</v>
@@ -6055,7 +6055,7 @@
         <v>2.38</v>
       </c>
       <c r="K75">
-        <v>1.28</v>
+        <v>1.2834000000000001</v>
       </c>
       <c r="L75">
         <v>271.47000000000003</v>
@@ -6126,7 +6126,7 @@
         <v>2.38</v>
       </c>
       <c r="K76">
-        <v>1.28</v>
+        <v>1.2834000000000001</v>
       </c>
       <c r="L76">
         <v>271.47000000000003</v>
@@ -6197,7 +6197,7 @@
         <v>2.4</v>
       </c>
       <c r="K77">
-        <v>4.8600000000000003</v>
+        <v>4.862099999999999</v>
       </c>
       <c r="L77">
         <v>246.61</v>
@@ -6268,7 +6268,7 @@
         <v>2.4</v>
       </c>
       <c r="K78">
-        <v>4.8600000000000003</v>
+        <v>4.862099999999999</v>
       </c>
       <c r="L78">
         <v>246.61</v>
@@ -6339,7 +6339,7 @@
         <v>2.4</v>
       </c>
       <c r="K79">
-        <v>4.8600000000000003</v>
+        <v>4.862099999999999</v>
       </c>
       <c r="L79">
         <v>246.61</v>
@@ -6410,7 +6410,7 @@
         <v>1.35</v>
       </c>
       <c r="K80">
-        <v>1.03</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="L80">
         <v>277.43</v>
@@ -6481,7 +6481,7 @@
         <v>1.35</v>
       </c>
       <c r="K81">
-        <v>1.03</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="L81">
         <v>277.43</v>
@@ -6552,7 +6552,7 @@
         <v>1.35</v>
       </c>
       <c r="K82">
-        <v>1.03</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="L82">
         <v>277.43</v>
@@ -6623,7 +6623,7 @@
         <v>1.23</v>
       </c>
       <c r="K83">
-        <v>4.12</v>
+        <v>4.1216000000000008</v>
       </c>
       <c r="L83">
         <v>240.54</v>
@@ -6694,7 +6694,7 @@
         <v>1.23</v>
       </c>
       <c r="K84">
-        <v>4.12</v>
+        <v>4.1216000000000008</v>
       </c>
       <c r="L84">
         <v>240.54</v>
@@ -6765,7 +6765,7 @@
         <v>1.23</v>
       </c>
       <c r="K85">
-        <v>4.12</v>
+        <v>4.1216000000000008</v>
       </c>
       <c r="L85">
         <v>240.54</v>
@@ -7475,7 +7475,7 @@
         <v>1.18</v>
       </c>
       <c r="K95">
-        <v>2.23</v>
+        <v>2.2334399999999999</v>
       </c>
       <c r="L95">
         <v>245</v>
@@ -7546,7 +7546,7 @@
         <v>1.18</v>
       </c>
       <c r="K96">
-        <v>2.23</v>
+        <v>2.2334399999999999</v>
       </c>
       <c r="L96">
         <v>245</v>
@@ -7617,7 +7617,7 @@
         <v>1.18</v>
       </c>
       <c r="K97">
-        <v>2.23</v>
+        <v>2.2334399999999999</v>
       </c>
       <c r="L97">
         <v>245</v>
@@ -7901,7 +7901,7 @@
         <v>1.6</v>
       </c>
       <c r="K101">
-        <v>0.94</v>
+        <v>0.94300000000000017</v>
       </c>
       <c r="L101">
         <v>234.53</v>
@@ -7972,7 +7972,7 @@
         <v>1.6</v>
       </c>
       <c r="K102">
-        <v>0.94</v>
+        <v>0.94300000000000017</v>
       </c>
       <c r="L102">
         <v>234.53</v>
@@ -8043,7 +8043,7 @@
         <v>1.6</v>
       </c>
       <c r="K103">
-        <v>0.94</v>
+        <v>0.94300000000000017</v>
       </c>
       <c r="L103">
         <v>234.53</v>

</xml_diff>